<commit_message>
Manually correct states in Partners clinic raw data
</commit_message>
<xml_diff>
--- a/data/Partners_raw/Clinical.xlsx
+++ b/data/Partners_raw/Clinical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\clients\PARTNERS\COVID\Schools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pjrule/Google Drive/Tufts/MGGG/covid-analysis/data/Partners_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{22DC4FF4-6862-4E61-BA6A-6E618B5EA8D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2FA0FB3-C314-A34E-9706-9E968344168E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19640" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClinicalSitesover5ksf (1)" sheetId="1" r:id="rId1"/>
@@ -1300,7 +1300,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2137,23 +2137,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>104</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>106</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>111</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>114</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>116</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>118</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>128</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>145</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>148</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>148</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>151</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>152</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>153</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>156</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>148</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>158</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>161</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>165</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>167</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>168</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>170</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>172</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>173</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>176</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>179</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>183</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>186</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>188</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>190</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>192</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>194</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>198</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>201</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>203</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>206</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>210</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>213</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>214</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>216</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>170</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>217</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>183</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>116</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>219</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>220</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>222</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>223</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>225</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>226</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>230</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>233</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>109</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>235</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>236</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>238</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>240</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>241</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>243</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>245</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>246</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>114</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>248</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>250</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>253</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>255</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>257</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>261</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>263</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>265</v>
       </c>
@@ -4314,13 +4314,13 @@
         <v>258</v>
       </c>
       <c r="C134" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
       <c r="D134" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>266</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>268</v>
       </c>
@@ -4342,13 +4342,13 @@
         <v>258</v>
       </c>
       <c r="C136" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
       <c r="D136" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>269</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>270</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>272</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>273</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>275</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>276</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>277</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>278</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>279</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>281</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>135</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>282</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>283</v>
       </c>
       <c r="C148" t="s">
-        <v>7</v>
+        <v>325</v>
       </c>
       <c r="D148" t="s">
         <v>127</v>
@@ -4528,7 +4528,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>284</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>135</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>285</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>288</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>289</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>290</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>291</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>116</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>292</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>167</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>116</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>116</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>170</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>170</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>225</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>116</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>295</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>299</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>301</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>183</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>302</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>304</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>305</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>306</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>308</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>310</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>313</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>315</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>317</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>320</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>167</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>322</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>266</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>266</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>275</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>266</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>275</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>266</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>266</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>323</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>266</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>266</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>326</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>217</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>183</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>148</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>328</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>330</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>331</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>333</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>335</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>337</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>339</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>341</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>343</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>109</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>344</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>109</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>109</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>348</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>109</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>351</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>352</v>
       </c>
       <c r="C210" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
       <c r="D210" t="s">
         <v>260</v>
@@ -5579,7 +5579,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>353</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>274</v>
       </c>
       <c r="C211" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
       <c r="D211" t="s">
         <v>260</v>
@@ -5596,7 +5596,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>354</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>131</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>358</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>128</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>359</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>148</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>148</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>148</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>148</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>148</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>148</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>148</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>360</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>167</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>165</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>167</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>361</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>364</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>367</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>370</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>371</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>373</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>375</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>377</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>379</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>380</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>381</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>382</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>384</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>386</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>388</v>
       </c>
@@ -6157,7 +6157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>390</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>391</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>392</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>393</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>395</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>397</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>213</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>399</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>400</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>183</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>402</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>405</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>406</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>344</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>333</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>410</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>412</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>410</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>414</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>417</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>109</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>419</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>421</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>423</v>
       </c>

</xml_diff>